<commit_message>
Application password support, some other minor fixes
For rm only, removed sending of header net.jazz.jfs.owning-context - doesn't seem to be needed for 7.x
More prep for type system quality checker, but no user code yet
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests_710.xlsx
+++ b/elmclient/tests/tests_710.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3109FFF9-C5A0-4C69-8F7A-2054E437A167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31A9C3E-AE07-4606-94AA-36861A04F314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7971" yWindow="2237" windowWidth="24686" windowHeight="15026" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="4149" yWindow="2100" windowWidth="24685" windowHeight="15026" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="233">
   <si>
     <t>oslc_rm:uses</t>
   </si>
@@ -721,6 +721,12 @@
   </si>
   <si>
     <t>rm:module=^"AMR Stakeholder Requirements Specification" and oslc:instanceShape='Stakeholder Requirement'</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>tests\results\rm101b.html</t>
   </si>
 </sst>
 </file>
@@ -1167,11 +1173,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
-  <dimension ref="A1:AH111"/>
+  <dimension ref="A1:AI111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1199,11 +1205,11 @@
     <col min="23" max="24" width="9.15234375" style="1"/>
     <col min="25" max="25" width="24.3828125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.15234375" style="1"/>
-    <col min="27" max="27" width="24.3046875" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.15234375" style="1"/>
+    <col min="27" max="28" width="24.3046875" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1286,22 +1292,25 @@
         <v>86</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>200</v>
       </c>
@@ -1344,9 +1353,9 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="AH3" s="17"/>
-    </row>
-    <row r="4" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="AI3" s="17"/>
+    </row>
+    <row r="4" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
         <v>79</v>
       </c>
@@ -1393,8 +1402,11 @@
       <c r="AA4" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="AB4" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
         <v>75</v>
       </c>
@@ -1437,7 +1449,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>208</v>
       </c>
@@ -1480,7 +1492,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>50</v>
       </c>
@@ -1511,7 +1523,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="8" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -1545,7 +1557,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="9" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B9" s="5" t="s">
         <v>75</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="10" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>75</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="11" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
         <v>75</v>
       </c>
@@ -1668,7 +1680,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="12" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>75</v>
       </c>
@@ -1713,7 +1725,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="13" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>221</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="14" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>99</v>
       </c>
@@ -1809,7 +1821,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="15" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>99</v>
       </c>
@@ -1857,7 +1869,7 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="16" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>99</v>
       </c>
@@ -4804,8 +4816,8 @@
       </c>
     </row>
     <row r="96" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="97" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="99" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="99" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="14" t="s">
         <v>202</v>
       </c>
@@ -4822,7 +4834,7 @@
       <c r="P99" s="15"/>
       <c r="Y99" s="16"/>
     </row>
-    <row r="100" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B100" s="14" t="s">
         <v>134</v>
       </c>
@@ -4863,11 +4875,11 @@
         <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
-      <c r="AB100" s="14" t="s">
+      <c r="AC100" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B101" s="14" t="s">
         <v>134</v>
       </c>
@@ -4909,11 +4921,11 @@
       <c r="Y101" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AC101" s="14" t="s">
+      <c r="AD101" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B102" s="14" t="s">
         <v>134</v>
       </c>
@@ -4955,14 +4967,14 @@
       <c r="Y102" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AC102" s="14" t="s">
+      <c r="AD102" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AE102" s="14" t="s">
+      <c r="AF102" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="103" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B103" s="14" t="s">
         <v>134</v>
       </c>
@@ -5001,11 +5013,11 @@
       <c r="Y103" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AD103" s="14" t="s">
+      <c r="AE103" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B104" s="14" t="s">
         <v>134</v>
       </c>
@@ -5047,11 +5059,11 @@
       <c r="Y104" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AC104" s="14" t="s">
+      <c r="AD104" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="105" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B105" s="14" t="s">
         <v>134</v>
       </c>
@@ -5093,14 +5105,14 @@
         <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
-      <c r="AB105" s="14" t="s">
+      <c r="AC105" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AE105" s="14" t="s">
+      <c r="AF105" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="106" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B106" s="14" t="s">
         <v>134</v>
       </c>
@@ -5139,14 +5151,14 @@
       <c r="Y106" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AC106" s="14" t="s">
+      <c r="AD106" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AE106" s="14" t="s">
+      <c r="AF106" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B107" s="14" t="s">
         <v>134</v>
       </c>
@@ -5188,14 +5200,14 @@
       <c r="Y107" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AC107" s="14" t="s">
+      <c r="AD107" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AE107" s="14" t="s">
+      <c r="AF107" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B108" s="14" t="s">
         <v>134</v>
       </c>
@@ -5237,11 +5249,11 @@
       <c r="Y108" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AC108" s="14" t="s">
+      <c r="AD108" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="109" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B109" s="14" t="s">
         <v>134</v>
       </c>
@@ -5280,11 +5292,11 @@
       <c r="Y109" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AD109" s="14" t="s">
+      <c r="AE109" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="110" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="I110" s="15"/>
       <c r="J110" s="15"/>
       <c r="K110" s="15"/>
@@ -5295,7 +5307,7 @@
       <c r="P110" s="15"/>
       <c r="Y110" s="16"/>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.4">
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>

</xml_diff>

<commit_message>
Various updates, tested oslcquery against 7.1
fixed spelling error cas.eys()
Started resources.py as a possible way of getting python objects for RM resources
Fixed various problems (including represet.py) caused by outdated use of rdm_types:ArtifactFormat - all replaced with rdf:type
Added customScenarios.py which comes with a built-in test for the API to start/stop custom scenarios
Added discover sequence in rm_basic_discovery.py - generates a html log of the discovery sequence from rootservices to configurations and services.xml
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests_710.xlsx
+++ b/elmclient/tests/tests_710.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31A9C3E-AE07-4606-94AA-36861A04F314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2853AD3-CB6E-4CE1-AAE6-9E744B5AFA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4149" yWindow="2100" windowWidth="24685" windowHeight="15026" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="2500" yWindow="110" windowWidth="28170" windowHeight="16500" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -216,9 +216,6 @@
     <t>All module artifacts in Text format</t>
   </si>
   <si>
-    <t>dcterms:title,rdm_types:ArtifactFormat,oslc:instanceShape</t>
-  </si>
-  <si>
     <t>Titles of All artifacts in a specific collection by identifier</t>
   </si>
   <si>
@@ -727,6 +724,9 @@
   </si>
   <si>
     <t>tests\results\rm101b.html</t>
+  </si>
+  <si>
+    <t>dcterms:title,rdf:type,oslc:instanceShape</t>
   </si>
 </sst>
 </file>
@@ -1175,41 +1175,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
   <dimension ref="A1:AI111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB4" sqref="AB4"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.3828125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.84375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.3046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.3046875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.15234375" style="1"/>
-    <col min="7" max="8" width="39.3828125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="61.84375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="54.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.1796875" style="1"/>
+    <col min="7" max="8" width="39.36328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="61.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="54.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.3046875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.15234375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="26.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.84375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="9.15234375" style="1"/>
-    <col min="25" max="25" width="24.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.15234375" style="1"/>
-    <col min="27" max="28" width="24.3046875" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.15234375" style="1"/>
+    <col min="13" max="13" width="22.26953125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.81640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9.1796875" style="1"/>
+    <col min="25" max="25" width="24.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.1796875" style="1"/>
+    <col min="27" max="28" width="24.26953125" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1220,19 +1220,19 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>30</v>
@@ -1241,10 +1241,10 @@
         <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>32</v>
@@ -1268,10 +1268,10 @@
         <v>34</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>10</v>
@@ -1289,39 +1289,39 @@
         <v>36</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1332,18 +1332,18 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="W2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y2" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -1355,9 +1355,9 @@
       <c r="P3" s="6"/>
       <c r="AI3" s="17"/>
     </row>
-    <row r="4" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="5">
         <v>101</v>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -1400,15 +1400,15 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="5">
         <f>C4+1</f>
@@ -1418,10 +1418,10 @@
         <v>2</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>8</v>
@@ -1449,12 +1449,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" ref="C6:C54" si="3">C5+1</f>
@@ -1492,12 +1492,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="3"/>
@@ -1523,12 +1523,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="3"/>
@@ -1557,9 +1557,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="3"/>
@@ -1600,9 +1600,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="3"/>
@@ -1615,7 +1615,7 @@
         <v>17</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1640,9 +1640,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" si="3"/>
@@ -1655,7 +1655,7 @@
         <v>17</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1680,9 +1680,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="3"/>
@@ -1692,7 +1692,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>41</v>
@@ -1725,12 +1725,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="3"/>
@@ -1743,7 +1743,7 @@
         <v>18</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>0</v>
@@ -1773,12 +1773,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" si="3"/>
@@ -1788,13 +1788,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -1821,12 +1821,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="15" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" si="3"/>
@@ -1839,7 +1839,7 @@
         <v>19</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>1</v>
@@ -1869,12 +1869,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="16" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" si="3"/>
@@ -1887,7 +1887,7 @@
         <v>20</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>2</v>
@@ -1917,22 +1917,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="17" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M17" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1957,9 +1957,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="18" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" si="3"/>
@@ -1994,9 +1994,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" si="3"/>
@@ -2031,9 +2031,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="20" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" si="3"/>
@@ -2071,9 +2071,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="21" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" si="3"/>
@@ -2083,10 +2083,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="M21" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2111,9 +2111,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="22" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" si="3"/>
@@ -2154,9 +2154,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" si="3"/>
@@ -2197,9 +2197,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" si="3"/>
@@ -2237,9 +2237,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" si="3"/>
@@ -2278,12 +2278,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" si="3"/>
@@ -2296,7 +2296,7 @@
         <v>44</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M26" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2322,12 +2322,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="27" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" si="3"/>
@@ -2340,10 +2340,10 @@
         <v>45</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="M27" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2368,12 +2368,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="28" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="5">
         <f t="shared" si="3"/>
@@ -2386,10 +2386,10 @@
         <v>60</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="M28" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2419,12 +2419,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="29" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
@@ -2437,10 +2437,10 @@
         <v>61</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="M29" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2468,12 +2468,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
@@ -2486,7 +2486,7 @@
         <v>59</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="M30" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2516,9 +2516,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
@@ -2534,7 +2534,7 @@
         <v>57</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="M31" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2559,9 +2559,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
@@ -2577,7 +2577,7 @@
         <v>57</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="M32" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2602,9 +2602,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="33" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
@@ -2614,10 +2614,10 @@
         <v>112</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M33" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2642,9 +2642,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="34" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
@@ -2654,17 +2654,17 @@
         <v>18</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tests\results\test131.csv</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q34" s="5" t="s">
         <v>11</v>
@@ -2685,9 +2685,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="35" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
@@ -2697,17 +2697,17 @@
         <v>94</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tests\results\test132.csv</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q35" s="5" t="s">
         <v>11</v>
@@ -2728,22 +2728,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="36" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F36" s="5">
         <v>1478</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I36" s="8"/>
       <c r="M36" s="6" t="str">
@@ -2751,13 +2751,13 @@
         <v>tests\results\test133.csv</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T36" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="U36" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="U36" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="V36" s="5" t="s">
         <v>12</v>
@@ -2775,9 +2775,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="37" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
@@ -2787,7 +2787,7 @@
         <v>739</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I37" s="8"/>
       <c r="M37" s="6" t="str">
@@ -2795,13 +2795,13 @@
         <v>tests\results\test134.csv</v>
       </c>
       <c r="Q37" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S37" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V37" s="5" t="s">
         <v>12</v>
@@ -2819,9 +2819,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="38" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
@@ -2831,7 +2831,7 @@
         <v>739</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I38" s="8"/>
       <c r="M38" s="6" t="str">
@@ -2839,13 +2839,13 @@
         <v>tests\results\test135.csv</v>
       </c>
       <c r="Q38" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S38" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V38" s="5" t="s">
         <v>12</v>
@@ -2863,9 +2863,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="39" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
@@ -2875,11 +2875,11 @@
         <v>51</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I39" s="8"/>
       <c r="K39" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M39" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2904,9 +2904,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="40" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
@@ -2916,16 +2916,16 @@
         <v>112</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>8</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M40" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2950,9 +2950,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="41" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
@@ -2962,10 +2962,10 @@
         <v>1</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I41" s="8"/>
       <c r="L41" s="6"/>
@@ -2992,9 +2992,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="42" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
@@ -3004,10 +3004,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I42" s="8"/>
       <c r="L42" s="6"/>
@@ -3034,9 +3034,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="43" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
@@ -3046,10 +3046,10 @@
         <v>5</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I43" s="8"/>
       <c r="L43" s="6"/>
@@ -3076,22 +3076,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="44" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F44" s="5">
         <v>1652</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I44" s="8"/>
       <c r="M44" s="6" t="str">
@@ -3099,13 +3099,13 @@
         <v>tests\results\test141.csv</v>
       </c>
       <c r="Q44" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U44" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="V44" s="5" t="s">
         <v>12</v>
@@ -3123,9 +3123,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="45" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
@@ -3135,7 +3135,7 @@
         <v>325</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I45" s="8"/>
       <c r="M45" s="6" t="str">
@@ -3143,13 +3143,13 @@
         <v>tests\results\test142.csv</v>
       </c>
       <c r="Q45" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="S45" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="R45" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="S45" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="V45" s="5" t="s">
         <v>12</v>
@@ -3167,9 +3167,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="46" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
@@ -3179,7 +3179,7 @@
         <v>744</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I46" s="8"/>
       <c r="M46" s="6" t="str">
@@ -3187,13 +3187,13 @@
         <v>tests\results\test143.csv</v>
       </c>
       <c r="Q46" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R46" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S46" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V46" s="5" t="s">
         <v>12</v>
@@ -3211,9 +3211,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="47" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C47" s="5">
         <f t="shared" si="3"/>
@@ -3223,7 +3223,7 @@
         <v>583</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I47" s="8"/>
       <c r="M47" s="6" t="str">
@@ -3231,18 +3231,18 @@
         <v>tests\results\test144.csv</v>
       </c>
       <c r="Q47" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R47" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="S47" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="S47" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
@@ -3252,10 +3252,10 @@
         <v>92</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J48" s="5" t="s">
         <v>8</v>
@@ -3284,9 +3284,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="49" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
@@ -3296,10 +3296,10 @@
         <v>62</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>8</v>
@@ -3328,9 +3328,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="50" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B50" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
@@ -3340,10 +3340,10 @@
         <v>92</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>8</v>
@@ -3372,9 +3372,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="51" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
@@ -3384,10 +3384,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>8</v>
@@ -3416,9 +3416,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="52" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
@@ -3428,10 +3428,10 @@
         <v>92</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>8</v>
@@ -3460,12 +3460,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
@@ -3475,10 +3475,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>8</v>
@@ -3507,9 +3507,9 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="54" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
@@ -3519,7 +3519,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>42</v>
@@ -3551,27 +3551,27 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="55" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B58" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58" s="9">
         <v>201</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F58" s="9">
         <v>16</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>8</v>
@@ -3593,25 +3593,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="59" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B59" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C59" s="9">
         <f>C58+1</f>
         <v>202</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F59" s="9">
         <v>9</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M59" s="13" t="str">
         <f t="shared" si="16"/>
@@ -3630,22 +3630,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="60" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B60" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C60" s="9">
         <f t="shared" ref="C60:C65" si="19">C59+1</f>
         <v>203</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F60" s="9">
         <v>4</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H60" s="9" t="s">
         <v>34</v>
@@ -3667,35 +3667,35 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="61" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B61" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C61" s="9">
         <f t="shared" si="19"/>
         <v>204</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F61" s="9">
         <v>30</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M61" s="13" t="str">
         <f t="shared" ref="M61:M62" si="21">"tests\results\test"&amp;C61&amp;".csv"</f>
         <v>tests\results\test204.csv</v>
       </c>
       <c r="Q61" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S61" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="R61" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S61" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W61" s="9" t="str">
         <f t="shared" si="17"/>
@@ -3710,41 +3710,41 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA61" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B62" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C62" s="9">
         <f t="shared" si="19"/>
         <v>205</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F62" s="9">
         <v>4</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M62" s="13" t="str">
         <f t="shared" si="21"/>
         <v>tests\results\test205.csv</v>
       </c>
       <c r="Q62" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R62" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S62" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="R62" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S62" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W62" s="9" t="str">
         <f t="shared" si="17"/>
@@ -3759,38 +3759,38 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="63" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B63" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C63" s="9">
         <f t="shared" si="19"/>
         <v>206</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F63" s="9">
         <v>27</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M63" s="13" t="str">
         <f>"tests\results\test"&amp;C62&amp;".csv"</f>
         <v>tests\results\test205.csv</v>
       </c>
       <c r="Q63" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R63" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S63" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="R63" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S63" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W63" s="9" t="str">
         <f t="shared" si="17"/>
@@ -3805,38 +3805,38 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="64" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B64" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C64" s="9">
         <f t="shared" si="19"/>
         <v>207</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F64" s="9">
         <v>22</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M64" s="13" t="str">
         <f>"tests\results\test"&amp;C63&amp;".csv"</f>
         <v>tests\results\test206.csv</v>
       </c>
       <c r="N64" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q64" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R64" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S64" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="R64" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S64" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W64" s="9" t="str">
         <f t="shared" si="17"/>
@@ -3851,38 +3851,38 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="65" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B65" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C65" s="9">
         <f t="shared" si="19"/>
         <v>208</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F65" s="9">
         <v>8</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M65" s="13" t="str">
         <f>"tests\results\test"&amp;C64&amp;".csv"</f>
         <v>tests\results\test207.csv</v>
       </c>
       <c r="P65" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q65" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R65" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S65" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="R65" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S65" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W65" s="9" t="str">
         <f t="shared" si="17"/>
@@ -3897,16 +3897,16 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="66" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M66" s="13"/>
       <c r="Q66" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R66" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S66" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="R66" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S66" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W66" s="9" t="str">
         <f t="shared" si="17"/>
@@ -3921,16 +3921,16 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="67" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M67" s="13"/>
       <c r="Q67" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R67" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S67" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="R67" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S67" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W67" s="9" t="str">
         <f t="shared" si="17"/>
@@ -3945,27 +3945,27 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="68" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="70" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B71" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71" s="4">
         <v>301</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F71" s="4">
         <v>89</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>8</v>
@@ -3975,7 +3975,7 @@
         <v>tests\results\test301.csv</v>
       </c>
       <c r="Q71" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W71" s="4" t="str">
         <f t="shared" ref="W71:X86" si="23">W$2</f>
@@ -3990,28 +3990,28 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA71" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="72" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B72" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C72" s="4">
         <f>C71+1</f>
         <v>302</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F72" s="4">
         <v>34</v>
       </c>
       <c r="G72" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I72" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>8</v>
@@ -4021,7 +4021,7 @@
         <v>tests\results\test302.csv</v>
       </c>
       <c r="Q72" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W72" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4036,25 +4036,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="73" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B73" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C73" s="4">
         <f t="shared" ref="C73:C82" si="25">C72+1</f>
         <v>303</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F73" s="4">
         <v>23</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>8</v>
@@ -4064,7 +4064,7 @@
         <v>tests\results\test303.csv</v>
       </c>
       <c r="Q73" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W73" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4079,25 +4079,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="74" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B74" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C74" s="4">
         <f t="shared" si="25"/>
         <v>304</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F74" s="4">
         <v>2</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>8</v>
@@ -4107,7 +4107,7 @@
         <v>tests\results\test304.csv</v>
       </c>
       <c r="Q74" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W74" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4122,35 +4122,35 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="75" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B75" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C75" s="4">
         <f t="shared" si="25"/>
         <v>305</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F75" s="4">
         <v>12</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M75" s="11" t="str">
         <f t="shared" si="22"/>
         <v>tests\results\test305.csv</v>
       </c>
       <c r="Q75" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W75" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4165,25 +4165,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="76" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B76" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76" s="4">
         <f t="shared" si="25"/>
         <v>306</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F76" s="4">
         <v>89</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>8</v>
@@ -4193,7 +4193,7 @@
         <v>tests\results\test306.csv</v>
       </c>
       <c r="Q76" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W76" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4208,25 +4208,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="77" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B77" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C77" s="4">
         <f t="shared" si="25"/>
         <v>307</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F77" s="4">
         <v>0</v>
       </c>
       <c r="G77" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I77" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="I77" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>8</v>
@@ -4236,7 +4236,7 @@
         <v>tests\results\test307.csv</v>
       </c>
       <c r="Q77" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W77" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4251,22 +4251,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="78" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B78" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C78" s="4">
         <f t="shared" si="25"/>
         <v>308</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F78" s="4">
         <v>23</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>8</v>
@@ -4276,10 +4276,10 @@
         <v>tests\results\test308.csv</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q78" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W78" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4294,22 +4294,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="79" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B79" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C79" s="4">
         <f t="shared" si="25"/>
         <v>309</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F79" s="4">
         <v>66</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>8</v>
@@ -4319,10 +4319,10 @@
         <v>tests\results\test309.csv</v>
       </c>
       <c r="P79" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q79" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W79" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4337,25 +4337,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="80" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B80" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C80" s="4">
         <f t="shared" si="25"/>
         <v>310</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F80" s="4">
         <v>38</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>8</v>
@@ -4365,7 +4365,7 @@
         <v>tests\results\test310.csv</v>
       </c>
       <c r="Q80" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W80" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4380,32 +4380,32 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="81" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B81" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C81" s="4">
         <f t="shared" si="25"/>
         <v>311</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F81" s="4">
         <v>1</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M81" s="11" t="str">
         <f t="shared" si="26"/>
         <v>tests\results\test311.csv</v>
       </c>
       <c r="Q81" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W81" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4420,22 +4420,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="82" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B82" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C82" s="4">
         <f t="shared" si="25"/>
         <v>312</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F82" s="4">
         <v>0</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>8</v>
@@ -4445,10 +4445,10 @@
         <v>tests\results\test312.csv</v>
       </c>
       <c r="N82" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q82" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W82" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4463,13 +4463,13 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA82" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="83" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M83" s="11"/>
       <c r="Q83" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W83" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4484,10 +4484,10 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="84" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M84" s="11"/>
       <c r="Q84" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W84" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4502,10 +4502,10 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="85" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M85" s="11"/>
       <c r="Q85" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W85" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4520,10 +4520,10 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="86" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M86" s="11"/>
       <c r="Q86" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W86" s="4" t="str">
         <f t="shared" si="23"/>
@@ -4538,29 +4538,29 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="87" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M87" s="11"/>
     </row>
-    <row r="89" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="90" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B90" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C90" s="3">
         <v>401</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F90" s="3">
         <v>26</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>35</v>
@@ -4585,22 +4585,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="91" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C91" s="3">
         <f>C90+1</f>
         <v>402</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F91" s="3">
         <v>5</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>34</v>
@@ -4625,22 +4625,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="92" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C92" s="3">
         <f t="shared" ref="C92:C95" si="31">C91+1</f>
         <v>403</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F92" s="3">
         <v>4</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>34</v>
@@ -4653,7 +4653,7 @@
         <v>tests\results\test403.csv</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W92" s="3" t="str">
         <f t="shared" si="28"/>
@@ -4668,25 +4668,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA92" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C93" s="3">
         <f t="shared" si="31"/>
         <v>404</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F93" s="3">
         <v>24</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>35</v>
@@ -4699,13 +4699,13 @@
         <v>tests\results\test404.csv</v>
       </c>
       <c r="Q93" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="R93" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="R93" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="S93" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W93" s="3" t="str">
         <f t="shared" si="28"/>
@@ -4720,28 +4720,28 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="94" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B94" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C94" s="3">
         <f t="shared" si="31"/>
         <v>405</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F94" s="3">
         <v>1</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I94" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J94" s="3" t="s">
         <v>8</v>
@@ -4751,7 +4751,7 @@
         <v>tests\results\test405.csv</v>
       </c>
       <c r="Q94" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W94" s="3" t="str">
         <f t="shared" si="28"/>
@@ -4766,28 +4766,28 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="95" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B95" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C95" s="3">
         <f t="shared" si="31"/>
         <v>406</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F95" s="3">
         <v>24</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>8</v>
@@ -4797,10 +4797,10 @@
         <v>tests\results\test406.csv</v>
       </c>
       <c r="Q95" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S95" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W95" s="3" t="str">
         <f t="shared" si="28"/>
@@ -4815,14 +4815,14 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="96" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="97" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="99" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="97" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="99" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I99" s="15"/>
       <c r="J99" s="15"/>
@@ -4834,15 +4834,15 @@
       <c r="P99" s="15"/>
       <c r="Y99" s="16"/>
     </row>
-    <row r="100" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B100" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C100" s="14">
         <v>1001</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I100" s="15"/>
       <c r="J100" s="15"/>
@@ -4876,12 +4876,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AC100" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="101" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="101" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B101" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C101" s="14">
         <f>C100+1</f>
@@ -4891,7 +4891,7 @@
         <v>738</v>
       </c>
       <c r="G101" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I101" s="15"/>
       <c r="J101" s="15"/>
@@ -4913,31 +4913,31 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W101" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X101" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X101" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y101" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD101" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="102" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B102" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C102" s="14">
         <f t="shared" ref="C102:C109" si="36">C101+1</f>
         <v>1003</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G102" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I102" s="15"/>
       <c r="J102" s="15"/>
@@ -4959,31 +4959,31 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W102" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X102" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X102" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y102" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD102" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF102" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="103" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="103" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B103" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C103" s="14">
         <f t="shared" si="36"/>
         <v>1004</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I103" s="15"/>
       <c r="J103" s="15"/>
@@ -5005,31 +5005,31 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W103" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X103" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X103" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y103" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AE103" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="104" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B104" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C104" s="14">
         <f t="shared" si="36"/>
         <v>1005</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I104" s="15"/>
       <c r="J104" s="15"/>
@@ -5051,28 +5051,28 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W104" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X104" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X104" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y104" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD104" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="105" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="105" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B105" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C105" s="14">
         <f t="shared" si="36"/>
         <v>1006</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
@@ -5106,22 +5106,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AC105" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF105" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="106" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B106" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C106" s="14">
         <f t="shared" si="36"/>
         <v>1007</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I106" s="15"/>
       <c r="J106" s="15"/>
@@ -5143,34 +5143,34 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W106" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X106" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X106" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y106" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD106" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF106" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="107" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B107" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C107" s="14">
         <f t="shared" si="36"/>
         <v>1008</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I107" s="15"/>
       <c r="J107" s="15"/>
@@ -5192,34 +5192,34 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W107" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X107" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X107" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y107" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD107" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF107" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="108" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B108" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C108" s="14">
         <f t="shared" si="36"/>
         <v>1009</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I108" s="15"/>
       <c r="J108" s="15"/>
@@ -5241,28 +5241,28 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W108" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X108" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X108" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y108" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD108" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="109" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="109" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B109" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C109" s="14">
         <f t="shared" si="36"/>
         <v>1010</v>
       </c>
       <c r="G109" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I109" s="15"/>
       <c r="J109" s="15"/>
@@ -5284,19 +5284,19 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W109" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="X109" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="X109" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="Y109" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AE109" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="110" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="110" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I110" s="15"/>
       <c r="J110" s="15"/>
       <c r="K110" s="15"/>
@@ -5307,7 +5307,7 @@
       <c r="P110" s="15"/>
       <c r="Y110" s="16"/>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.35">
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>

</xml_diff>